<commit_message>
Adding consent form and correcting a mistake in the Materiale file
</commit_message>
<xml_diff>
--- a/materiale.xlsx
+++ b/materiale.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au645888_uni_au_dk/Documents/Alting/Lingvistik/Projekter/arithmetics_project/arithmetics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="878" documentId="11_AD4D1D646341095ACB70000305D6FDD8683EDF08" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E46AD89-AC79-4087-ACDB-EE3E181C5765}"/>
+  <xr:revisionPtr revIDLastSave="879" documentId="11_AD4D1D646341095ACB70000305D6FDD8683EDF08" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E8291DF-B3A9-4174-BD3B-4666A0B9CDEC}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1226,7 +1226,7 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1324,7 +1324,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="5">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="H3" s="5">
         <v>58</v>

</xml_diff>

<commit_message>
Adding demographics and email-page. Finishing touches on instructions.
</commit_message>
<xml_diff>
--- a/materiale.xlsx
+++ b/materiale.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au645888_uni_au_dk/Documents/Alting/Lingvistik/Projekter/arithmetics_project/arithmetics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="879" documentId="11_AD4D1D646341095ACB70000305D6FDD8683EDF08" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E8291DF-B3A9-4174-BD3B-4666A0B9CDEC}"/>
+  <xr:revisionPtr revIDLastSave="887" documentId="11_AD4D1D646341095ACB70000305D6FDD8683EDF08" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{386A14D2-DB42-4931-8EE6-826109E2BF0B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="128">
   <si>
     <t>36 / 6 =</t>
   </si>
@@ -848,6 +848,45 @@
   </si>
   <si>
     <t>math_BL</t>
+  </si>
+  <si>
+    <t>Manden bar på kurven med varerne, som var</t>
+  </si>
+  <si>
+    <t>Moren tændte lysene på juletræet, som var</t>
+  </si>
+  <si>
+    <t>Direktøren modtog beskeden om leverancerne, som var</t>
+  </si>
+  <si>
+    <t>Cyklisten vrissede over grenene på cykelstien, som var</t>
+  </si>
+  <si>
+    <t>Den studerende læste bøgerne om emnet, som var</t>
+  </si>
+  <si>
+    <t>Ministeren forklarede hensigten med reformerne, som var</t>
+  </si>
+  <si>
+    <t>Arkæologen fremviste stenen med inskriptionerne, som var</t>
+  </si>
+  <si>
+    <t>Kæresten medbragte kassen med bøgerne, som var</t>
+  </si>
+  <si>
+    <t>Brandmanden slukkede branden i bygningerne, som var</t>
+  </si>
+  <si>
+    <t>Pædagogen roste tegningen af kaninerne, som var</t>
+  </si>
+  <si>
+    <t>Præsidenten talte om problemerne med inflationen, som var</t>
+  </si>
+  <si>
+    <t>Formanden deltog i mødet om nedskæringerne, som var</t>
+  </si>
+  <si>
+    <t>Sælgeren fremviste varerne fra firmaet, som var</t>
   </si>
 </sst>
 </file>
@@ -1223,10 +1262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2061,6 +2100,110 @@
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
     </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding finished materiale file
</commit_message>
<xml_diff>
--- a/materiale.xlsx
+++ b/materiale.xlsx
@@ -5,27 +5,36 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au645888_uni_au_dk/Documents/Alting/Lingvistik/Projekter/arithmetics_project/arithmetics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au645888_uni_au_dk/Documents/Alting/Lingvistik/Projekter/arithmetics_project/choosing_sentences/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="887" documentId="11_AD4D1D646341095ACB70000305D6FDD8683EDF08" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{386A14D2-DB42-4931-8EE6-826109E2BF0B}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{0F660437-4ADA-4AC9-B8DB-E5BC948AB845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A11769BD-A41C-413A-B89D-B66417C92053}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
   <si>
     <t>36 / 6 =</t>
   </si>
@@ -599,15 +608,6 @@
     <t>Kommisionen takkede kilden til donationerne, som var</t>
   </si>
   <si>
-    <t>Turistguiden fortalte om klokkerne i kirketårnet, som var</t>
-  </si>
-  <si>
-    <t>Forskeren kritiserede metoderne i studiet, som var</t>
-  </si>
-  <si>
-    <t>Ægteparret læste artiklerne i avisen, som var</t>
-  </si>
-  <si>
     <t>Husejeren gemte brevene fra kontoret, som var</t>
   </si>
   <si>
@@ -626,27 +626,9 @@
     <t>Vinduespudseren polerede vinduerne i bygningen, som var</t>
   </si>
   <si>
-    <t>Viceværten vaskede trapperne i opgangen, som var</t>
-  </si>
-  <si>
     <t>Aktivisten demonstrerede mod forureningen af søerne, som var</t>
   </si>
   <si>
-    <t>Journalisten skrev om kampene i grænseregionen, som var</t>
-  </si>
-  <si>
-    <t>Gartneren vandede tomaterne i drivhuset, som var</t>
-  </si>
-  <si>
-    <t>Pigen glædede sig til udflugterne i ferien, som var</t>
-  </si>
-  <si>
-    <t>Sekretæren afventede dokumenterne fra partnerselskabet, som var</t>
-  </si>
-  <si>
-    <t>Forfatteren forkastede afsnittene om togrejsen, som var</t>
-  </si>
-  <si>
     <t>Danseren øvede trinene til forestillingen, som var</t>
   </si>
   <si>
@@ -665,9 +647,6 @@
     <t>Spekulanten solgte aktierne i firmaet, som var</t>
   </si>
   <si>
-    <t>Drengen tænkte på festerne med klassen, som var</t>
-  </si>
-  <si>
     <t>43 - 27 =</t>
   </si>
   <si>
@@ -856,12 +835,6 @@
     <t>Moren tændte lysene på juletræet, som var</t>
   </si>
   <si>
-    <t>Direktøren modtog beskeden om leverancerne, som var</t>
-  </si>
-  <si>
-    <t>Cyklisten vrissede over grenene på cykelstien, som var</t>
-  </si>
-  <si>
     <t>Den studerende læste bøgerne om emnet, som var</t>
   </si>
   <si>
@@ -878,9 +851,6 @@
   </si>
   <si>
     <t>Pædagogen roste tegningen af kaninerne, som var</t>
-  </si>
-  <si>
-    <t>Præsidenten talte om problemerne med inflationen, som var</t>
   </si>
   <si>
     <t>Formanden deltog i mødet om nedskæringerne, som var</t>
@@ -893,7 +863,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -919,8 +889,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -930,12 +907,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -961,27 +932,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1262,16 +1232,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q41"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="54.90625" customWidth="1"/>
+    <col min="2" max="2" width="57.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.26953125" customWidth="1"/>
     <col min="4" max="4" width="15.08984375" customWidth="1"/>
     <col min="5" max="5" width="9.6328125" customWidth="1"/>
@@ -1286,39 +1256,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>111</v>
+      <c r="A1" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1330,54 +1301,54 @@
       <c r="E2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>5</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>8</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>6</v>
       </c>
-      <c r="I2" s="4"/>
+      <c r="I2" s="5"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3" s="5">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="2">
         <v>30</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="2">
         <v>76</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="2">
         <v>58</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>38</v>
+      <c r="B4" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>29</v>
@@ -1388,56 +1359,56 @@
       <c r="E4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>16</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>2</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>69</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="I4" s="5"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" s="5">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>63</v>
+      </c>
+      <c r="G5" s="2">
         <v>39</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="5">
-        <v>63</v>
-      </c>
-      <c r="G5" s="5">
-        <v>39</v>
-      </c>
-      <c r="H5" s="5">
+      <c r="H5" s="2">
         <v>74</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -1446,216 +1417,216 @@
       <c r="E6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>8</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>42</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>59</v>
       </c>
-      <c r="I6" s="8"/>
+      <c r="I6" s="10"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" s="5">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2">
+        <v>28</v>
+      </c>
+      <c r="G7" s="2">
+        <v>49</v>
+      </c>
+      <c r="H7" s="2">
+        <v>52</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2">
+        <v>15</v>
+      </c>
+      <c r="G8" s="2">
+        <v>31</v>
+      </c>
+      <c r="H8" s="2">
+        <v>34</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="2">
+        <v>24</v>
+      </c>
+      <c r="G9" s="2">
+        <v>63</v>
+      </c>
+      <c r="H9" s="2">
+        <v>7</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="5">
-        <v>28</v>
-      </c>
-      <c r="G7" s="5">
-        <v>49</v>
-      </c>
-      <c r="H7" s="5">
+      <c r="C10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="2">
+        <v>11</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>60</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="2">
+        <v>37</v>
+      </c>
+      <c r="G11" s="2">
+        <v>29</v>
+      </c>
+      <c r="H11" s="2">
+        <v>38</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="2">
+        <v>38</v>
+      </c>
+      <c r="G12" s="2">
+        <v>22</v>
+      </c>
+      <c r="H12" s="2">
+        <v>72</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" s="9">
-        <v>7</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="9">
-        <v>15</v>
-      </c>
-      <c r="G8" s="9">
-        <v>31</v>
-      </c>
-      <c r="H8" s="9">
-        <v>34</v>
-      </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="D13" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="2">
+        <v>37</v>
+      </c>
+      <c r="G13" s="2">
         <v>13</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="5">
-        <v>24</v>
-      </c>
-      <c r="G9" s="5">
-        <v>63</v>
-      </c>
-      <c r="H9" s="5">
-        <v>7</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A10" s="9">
-        <v>9</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="9">
-        <v>11</v>
-      </c>
-      <c r="G10" s="9">
-        <v>1</v>
-      </c>
-      <c r="H10" s="9">
-        <v>60</v>
-      </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="5">
-        <v>37</v>
-      </c>
-      <c r="G11" s="5">
-        <v>29</v>
-      </c>
-      <c r="H11" s="5">
-        <v>38</v>
-      </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12" s="9">
-        <v>11</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="9">
-        <v>38</v>
-      </c>
-      <c r="G12" s="9">
-        <v>22</v>
-      </c>
-      <c r="H12" s="9">
-        <v>72</v>
-      </c>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="5">
-        <v>37</v>
-      </c>
-      <c r="G13" s="5">
-        <v>13</v>
-      </c>
-      <c r="H13" s="5">
+      <c r="H13" s="2">
         <v>16</v>
       </c>
       <c r="I13" s="13"/>
@@ -1663,546 +1634,616 @@
       <c r="K13" s="12"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A14" s="9">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="11" t="s">
+      <c r="B14" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="2">
         <v>55</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="2">
         <v>27</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="2">
         <v>31</v>
       </c>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" s="5">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>48</v>
+      <c r="B15" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="5">
+        <v>56</v>
+      </c>
+      <c r="F15" s="2">
         <v>80</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="2">
         <v>74</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="2">
         <v>17</v>
       </c>
-      <c r="I15" s="12"/>
+      <c r="I15" s="6"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A16">
+      <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>106</v>
+      <c r="B16" s="7" t="s">
+        <v>96</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="9">
+        <v>59</v>
+      </c>
+      <c r="F16" s="2">
         <v>23</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="2">
         <v>41</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="2">
         <v>27</v>
       </c>
-      <c r="I16" s="14"/>
+      <c r="I16" s="6"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
+      <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="2">
+      <c r="B17" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="7">
         <v>28</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="7">
         <v>22</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="7">
         <v>27</v>
       </c>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18">
+      <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>50</v>
+      <c r="B18" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="9">
+        <v>65</v>
+      </c>
+      <c r="F18" s="2">
         <v>86</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="2">
         <v>88</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="2">
         <v>20</v>
       </c>
-      <c r="I18" s="14"/>
+      <c r="I18" s="6"/>
       <c r="J18" s="14"/>
       <c r="K18" s="14"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
+      <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" s="2">
+      <c r="B19" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="7">
         <v>62</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="7">
         <v>65</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="7">
         <v>28</v>
       </c>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20">
+      <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>51</v>
+      <c r="B20" s="7" t="s">
+        <v>108</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E20" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="2">
+        <v>48</v>
+      </c>
+      <c r="G20" s="2">
         <v>81</v>
       </c>
-      <c r="F20" s="9">
-        <v>48</v>
-      </c>
-      <c r="G20" s="9">
-        <v>81</v>
-      </c>
-      <c r="H20" s="9">
+      <c r="H20" s="2">
         <v>63</v>
       </c>
-      <c r="I20" s="14"/>
+      <c r="I20" s="6"/>
       <c r="J20" s="14"/>
       <c r="K20" s="14"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
+      <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="F21" s="2">
+      <c r="B21" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="7">
         <v>13</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="7">
         <v>24</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="7">
         <v>42</v>
       </c>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22">
+      <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>54</v>
+      <c r="B22" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" s="9">
+        <v>77</v>
+      </c>
+      <c r="F22" s="2">
         <v>0</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="2">
         <v>50</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="2">
         <v>57</v>
       </c>
-      <c r="I22" s="14"/>
+      <c r="I22" s="6"/>
       <c r="J22" s="14"/>
       <c r="K22" s="14"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
+      <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="F23" s="2">
+      <c r="B23" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="7">
         <v>96</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="7">
         <v>45</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="7">
         <v>48</v>
       </c>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24">
+      <c r="A24" s="7">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
-        <v>56</v>
+      <c r="B24" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24" s="9">
+        <v>83</v>
+      </c>
+      <c r="F24" s="2">
         <v>64</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="2">
         <v>46</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="2">
         <v>4</v>
       </c>
-      <c r="I24" s="14"/>
+      <c r="I24" s="6"/>
       <c r="J24" s="14"/>
       <c r="K24" s="14"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
+      <c r="A25" s="7">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="F25" s="2">
+      <c r="B25" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="7">
         <v>112</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="7">
         <v>34</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="7">
         <v>20</v>
       </c>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26">
+      <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>58</v>
+      <c r="B26" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F26">
+        <v>90</v>
+      </c>
+      <c r="F26" s="7">
         <v>1</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="7">
         <v>48</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="7">
         <v>35</v>
       </c>
-      <c r="I26" s="14"/>
+      <c r="I26" s="8"/>
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="2">
+      <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27" s="15" t="s">
+      <c r="B27" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="7">
         <v>9</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="7">
         <v>15</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="7">
         <v>60</v>
       </c>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28">
+      <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
-        <v>60</v>
+      <c r="B28" s="7" t="s">
+        <v>110</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F28">
+        <v>95</v>
+      </c>
+      <c r="F28" s="7">
         <v>30</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="7">
         <v>22</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="7">
         <v>24</v>
       </c>
-      <c r="I28" s="14"/>
+      <c r="I28" s="8"/>
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="2">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>115</v>
-      </c>
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>116</v>
-      </c>
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="2">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>117</v>
-      </c>
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="2">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="2">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="2">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="2">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="2">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>127</v>
-      </c>
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="8"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="8"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="8"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>